<commit_message>
Update integration logic (name-based merge) and add PDF generation
</commit_message>
<xml_diff>
--- a/学習記録_統合_2026-02-12.xlsx
+++ b/学習記録_統合_2026-02-12.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoyamahiroki/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoyamahiroki/Desktop/3rdFebDrill/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889613C2-4C79-2E43-9BD5-0D39F326FBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40AAF21C-75C5-3A4C-ABD7-DCA4488CC4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="600" windowWidth="32840" windowHeight="19440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -964,178 +964,179 @@
     <t>谷川　颯</t>
   </si>
   <si>
+    <t>谷村　眞</t>
+  </si>
+  <si>
+    <t>玉城　有珠</t>
+  </si>
+  <si>
+    <t>田村　颯真</t>
+  </si>
+  <si>
+    <t>田和　莉瑚</t>
+  </si>
+  <si>
+    <t>辻井　紗季</t>
+  </si>
+  <si>
+    <t>釣島　里奈</t>
+  </si>
+  <si>
+    <t>寺田　天幸</t>
+  </si>
+  <si>
+    <t>中間　彪賀</t>
+  </si>
+  <si>
+    <t>中村　光鈴</t>
+  </si>
+  <si>
+    <t>中山　凜大</t>
+  </si>
+  <si>
+    <t>成井　惺一</t>
+  </si>
+  <si>
+    <t>西薗　蒼真</t>
+  </si>
+  <si>
+    <t>西村　有祐美</t>
+  </si>
+  <si>
+    <t>西山　泰生</t>
+  </si>
+  <si>
+    <t>P23075</t>
+  </si>
+  <si>
+    <t>野間　匠悟</t>
+  </si>
+  <si>
+    <t>野村　奈月香</t>
+  </si>
+  <si>
+    <t>野村　優輝</t>
+  </si>
+  <si>
+    <t>畑中　結衣</t>
+  </si>
+  <si>
+    <t>八田　翔真</t>
+  </si>
+  <si>
+    <t>八田　凌雅</t>
+  </si>
+  <si>
+    <t>福岡　健太</t>
+  </si>
+  <si>
+    <t>福本　芽生</t>
+  </si>
+  <si>
+    <t>P23086</t>
+  </si>
+  <si>
+    <t>藤原　暖子</t>
+  </si>
+  <si>
+    <t>舟木　希実</t>
+  </si>
+  <si>
+    <t>細川　光尚</t>
+  </si>
+  <si>
+    <t>細川　瑠希</t>
+  </si>
+  <si>
+    <t>本田　遥人</t>
+  </si>
+  <si>
+    <t>桝本　晴輝</t>
+  </si>
+  <si>
+    <t>松浦　健佑</t>
+  </si>
+  <si>
+    <t>松﨑　優寿花</t>
+  </si>
+  <si>
+    <t>松田　陽翔</t>
+  </si>
+  <si>
+    <t>松村　心羽</t>
+  </si>
+  <si>
+    <t>松本　渉</t>
+  </si>
+  <si>
+    <t>松山　昊生</t>
+  </si>
+  <si>
+    <t>萬代　喬哉</t>
+  </si>
+  <si>
+    <t>南　柊哉</t>
+  </si>
+  <si>
+    <t>村田　弥咲</t>
+  </si>
+  <si>
+    <t>森澤　澪</t>
+  </si>
+  <si>
+    <t>森田　悠太</t>
+  </si>
+  <si>
+    <t>森野　のい</t>
+  </si>
+  <si>
+    <t>保田　美咲</t>
+  </si>
+  <si>
+    <t>山岡　倫也</t>
+  </si>
+  <si>
+    <t>山口　美優</t>
+  </si>
+  <si>
+    <t>山田　蒼</t>
+  </si>
+  <si>
+    <t>山田　蒼絃</t>
+  </si>
+  <si>
+    <t>山田　有香</t>
+  </si>
+  <si>
+    <t>山中　優光</t>
+  </si>
+  <si>
+    <t>山本　あやめ</t>
+  </si>
+  <si>
+    <t>山本　真実</t>
+  </si>
+  <si>
+    <t>山本　優菜</t>
+  </si>
+  <si>
+    <t>湯浅　愛唯</t>
+  </si>
+  <si>
+    <t>吉澤　塁唯</t>
+  </si>
+  <si>
+    <t>吉田　勇貴</t>
+  </si>
+  <si>
+    <t>吉仲　花凜</t>
+  </si>
+  <si>
+    <t>芳本　脩吾</t>
+  </si>
+  <si>
     <t>P23054</t>
-  </si>
-  <si>
-    <t>谷村　眞</t>
-  </si>
-  <si>
-    <t>玉城　有珠</t>
-  </si>
-  <si>
-    <t>田村　颯真</t>
-  </si>
-  <si>
-    <t>田和　莉瑚</t>
-  </si>
-  <si>
-    <t>辻井　紗季</t>
-  </si>
-  <si>
-    <t>釣島　里奈</t>
-  </si>
-  <si>
-    <t>寺田　天幸</t>
-  </si>
-  <si>
-    <t>中間　彪賀</t>
-  </si>
-  <si>
-    <t>中村　光鈴</t>
-  </si>
-  <si>
-    <t>中山　凜大</t>
-  </si>
-  <si>
-    <t>成井　惺一</t>
-  </si>
-  <si>
-    <t>西薗　蒼真</t>
-  </si>
-  <si>
-    <t>西村　有祐美</t>
-  </si>
-  <si>
-    <t>西山　泰生</t>
-  </si>
-  <si>
-    <t>P23075</t>
-  </si>
-  <si>
-    <t>野間　匠悟</t>
-  </si>
-  <si>
-    <t>野村　奈月香</t>
-  </si>
-  <si>
-    <t>野村　優輝</t>
-  </si>
-  <si>
-    <t>畑中　結衣</t>
-  </si>
-  <si>
-    <t>八田　翔真</t>
-  </si>
-  <si>
-    <t>八田　凌雅</t>
-  </si>
-  <si>
-    <t>福岡　健太</t>
-  </si>
-  <si>
-    <t>福本　芽生</t>
-  </si>
-  <si>
-    <t>P23086</t>
-  </si>
-  <si>
-    <t>藤原　暖子</t>
-  </si>
-  <si>
-    <t>舟木　希実</t>
-  </si>
-  <si>
-    <t>細川　光尚</t>
-  </si>
-  <si>
-    <t>細川　瑠希</t>
-  </si>
-  <si>
-    <t>本田　遥人</t>
-  </si>
-  <si>
-    <t>桝本　晴輝</t>
-  </si>
-  <si>
-    <t>松浦　健佑</t>
-  </si>
-  <si>
-    <t>松﨑　優寿花</t>
-  </si>
-  <si>
-    <t>松田　陽翔</t>
-  </si>
-  <si>
-    <t>松村　心羽</t>
-  </si>
-  <si>
-    <t>松本　渉</t>
-  </si>
-  <si>
-    <t>松山　昊生</t>
-  </si>
-  <si>
-    <t>萬代　喬哉</t>
-  </si>
-  <si>
-    <t>南　柊哉</t>
-  </si>
-  <si>
-    <t>村田　弥咲</t>
-  </si>
-  <si>
-    <t>森澤　澪</t>
-  </si>
-  <si>
-    <t>森田　悠太</t>
-  </si>
-  <si>
-    <t>森野　のい</t>
-  </si>
-  <si>
-    <t>保田　美咲</t>
-  </si>
-  <si>
-    <t>山岡　倫也</t>
-  </si>
-  <si>
-    <t>山口　美優</t>
-  </si>
-  <si>
-    <t>山田　蒼</t>
-  </si>
-  <si>
-    <t>山田　蒼絃</t>
-  </si>
-  <si>
-    <t>山田　有香</t>
-  </si>
-  <si>
-    <t>山中　優光</t>
-  </si>
-  <si>
-    <t>山本　あやめ</t>
-  </si>
-  <si>
-    <t>山本　真実</t>
-  </si>
-  <si>
-    <t>山本　優菜</t>
-  </si>
-  <si>
-    <t>湯浅　愛唯</t>
-  </si>
-  <si>
-    <t>吉澤　塁唯</t>
-  </si>
-  <si>
-    <t>吉田　勇貴</t>
-  </si>
-  <si>
-    <t>吉仲　花凜</t>
-  </si>
-  <si>
-    <t>芳本　脩吾</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -1177,7 +1178,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1187,6 +1188,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1227,7 +1240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1240,14 +1253,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1561,135 +1583,135 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7">
+      <c r="C1" s="11">
         <v>46055</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="7">
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11">
         <v>46056</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="7">
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="11">
         <v>46057</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="7">
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="11">
         <v>46058</v>
       </c>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="7">
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="11">
         <v>46062</v>
       </c>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="7">
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="10"/>
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="10"/>
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="11">
         <v>46065</v>
       </c>
-      <c r="AK1" s="6"/>
-      <c r="AL1" s="6"/>
-      <c r="AM1" s="6"/>
-      <c r="AN1" s="6"/>
-      <c r="AO1" s="6"/>
-      <c r="AP1" s="6"/>
-      <c r="AQ1" s="6"/>
-      <c r="AR1" s="6"/>
+      <c r="AK1" s="10"/>
+      <c r="AL1" s="10"/>
+      <c r="AM1" s="10"/>
+      <c r="AN1" s="10"/>
+      <c r="AO1" s="10"/>
+      <c r="AP1" s="10"/>
+      <c r="AQ1" s="10"/>
+      <c r="AR1" s="10"/>
     </row>
     <row r="2" spans="1:44">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6" t="s">
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6" t="s">
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6" t="s">
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6" t="s">
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6" t="s">
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6" t="s">
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6" t="s">
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="AE2" s="6"/>
-      <c r="AF2" s="6"/>
-      <c r="AG2" s="6" t="s">
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AH2" s="6"/>
-      <c r="AI2" s="6"/>
-      <c r="AJ2" s="6" t="s">
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="AK2" s="6"/>
-      <c r="AL2" s="6"/>
-      <c r="AM2" s="6" t="s">
+      <c r="AK2" s="10"/>
+      <c r="AL2" s="10"/>
+      <c r="AM2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="AN2" s="6"/>
-      <c r="AO2" s="6"/>
-      <c r="AP2" s="6" t="s">
+      <c r="AN2" s="10"/>
+      <c r="AO2" s="10"/>
+      <c r="AP2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AQ2" s="6"/>
-      <c r="AR2" s="6"/>
+      <c r="AQ2" s="10"/>
+      <c r="AR2" s="10"/>
     </row>
     <row r="3" spans="1:44">
       <c r="B3" s="1"/>
@@ -31468,10 +31490,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S115"/>
+  <dimension ref="A1:S114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="M56" sqref="A1:M56"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="P60" sqref="P60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -31479,6 +31501,7 @@
     <col min="1" max="1" width="5.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" customWidth="1"/>
     <col min="10" max="10" width="11.1640625" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="20" customHeight="1">
@@ -31566,10 +31589,10 @@
       <c r="M5" s="2">
         <v>39</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="P5" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="Q5" s="8" t="s">
+      <c r="Q5" s="9" t="s">
         <v>238</v>
       </c>
     </row>
@@ -31610,10 +31633,10 @@
       <c r="M6" s="2">
         <v>39</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="P6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="Q6" s="8" t="s">
+      <c r="Q6" s="6" t="s">
         <v>239</v>
       </c>
       <c r="R6" s="2" t="s">
@@ -31660,10 +31683,10 @@
       <c r="M7" s="2">
         <v>39</v>
       </c>
-      <c r="P7" s="8" t="s">
+      <c r="P7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="8" t="s">
+      <c r="Q7" s="6" t="s">
         <v>240</v>
       </c>
       <c r="R7" s="2" t="s">
@@ -31710,10 +31733,10 @@
       <c r="M8" s="2">
         <v>40</v>
       </c>
-      <c r="P8" s="8" t="s">
+      <c r="P8" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="Q8" s="8" t="s">
+      <c r="Q8" s="7" t="s">
         <v>242</v>
       </c>
       <c r="R8" s="2"/>
@@ -31756,10 +31779,10 @@
       <c r="M9" s="2">
         <v>40</v>
       </c>
-      <c r="P9" s="8" t="s">
+      <c r="P9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="Q9" s="8" t="s">
+      <c r="Q9" s="6" t="s">
         <v>243</v>
       </c>
       <c r="R9" s="2" t="s">
@@ -31806,10 +31829,10 @@
       <c r="M10" s="2">
         <v>40</v>
       </c>
-      <c r="P10" s="8" t="s">
+      <c r="P10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Q10" s="8" t="s">
+      <c r="Q10" s="6" t="s">
         <v>244</v>
       </c>
       <c r="R10" s="2" t="s">
@@ -31856,10 +31879,10 @@
       <c r="M11" s="2">
         <v>41</v>
       </c>
-      <c r="P11" s="8" t="s">
+      <c r="P11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Q11" s="8" t="s">
+      <c r="Q11" s="6" t="s">
         <v>245</v>
       </c>
       <c r="R11" s="2" t="s">
@@ -31906,10 +31929,10 @@
       <c r="M12" s="2">
         <v>41</v>
       </c>
-      <c r="P12" s="8" t="s">
+      <c r="P12" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="Q12" s="8" t="s">
+      <c r="Q12" s="6" t="s">
         <v>247</v>
       </c>
       <c r="R12" s="2" t="s">
@@ -31956,10 +31979,10 @@
       <c r="M13" s="2">
         <v>42</v>
       </c>
-      <c r="P13" s="8" t="s">
+      <c r="P13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="Q13" s="8" t="s">
+      <c r="Q13" s="6" t="s">
         <v>248</v>
       </c>
       <c r="R13" s="2" t="s">
@@ -32006,10 +32029,10 @@
       <c r="M14" s="2">
         <v>42</v>
       </c>
-      <c r="P14" s="8" t="s">
+      <c r="P14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="Q14" s="8" t="s">
+      <c r="Q14" s="7" t="s">
         <v>249</v>
       </c>
       <c r="R14" s="2"/>
@@ -32052,10 +32075,10 @@
       <c r="M15" s="2">
         <v>43</v>
       </c>
-      <c r="P15" s="8" t="s">
+      <c r="P15" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="Q15" s="8" t="s">
+      <c r="Q15" s="6" t="s">
         <v>250</v>
       </c>
       <c r="R15" s="2" t="s">
@@ -32102,10 +32125,10 @@
       <c r="M16" s="2">
         <v>43</v>
       </c>
-      <c r="P16" s="8" t="s">
+      <c r="P16" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="Q16" s="8" t="s">
+      <c r="Q16" s="6" t="s">
         <v>251</v>
       </c>
       <c r="R16" s="2" t="s">
@@ -32152,10 +32175,10 @@
       <c r="M17" s="2">
         <v>43</v>
       </c>
-      <c r="P17" s="8" t="s">
+      <c r="P17" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="Q17" s="8" t="s">
+      <c r="Q17" s="6" t="s">
         <v>252</v>
       </c>
       <c r="R17" s="2" t="s">
@@ -32202,10 +32225,10 @@
       <c r="M18" s="2">
         <v>43</v>
       </c>
-      <c r="P18" s="8" t="s">
+      <c r="P18" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="Q18" s="8" t="s">
+      <c r="Q18" s="6" t="s">
         <v>253</v>
       </c>
       <c r="R18" s="2" t="s">
@@ -32252,10 +32275,10 @@
       <c r="M19" s="2">
         <v>43</v>
       </c>
-      <c r="P19" s="8" t="s">
+      <c r="P19" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="Q19" s="8" t="s">
+      <c r="Q19" s="6" t="s">
         <v>254</v>
       </c>
       <c r="R19" s="2" t="s">
@@ -32302,10 +32325,10 @@
       <c r="M20" s="2">
         <v>44</v>
       </c>
-      <c r="P20" s="8" t="s">
+      <c r="P20" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="Q20" s="8" t="s">
+      <c r="Q20" s="6" t="s">
         <v>255</v>
       </c>
       <c r="R20" s="2" t="s">
@@ -32352,10 +32375,10 @@
       <c r="M21" s="2">
         <v>44</v>
       </c>
-      <c r="P21" s="8" t="s">
+      <c r="P21" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="Q21" s="8" t="s">
+      <c r="Q21" s="6" t="s">
         <v>256</v>
       </c>
       <c r="R21" s="2" t="s">
@@ -32402,10 +32425,10 @@
       <c r="M22" s="2">
         <v>45</v>
       </c>
-      <c r="P22" s="8" t="s">
+      <c r="P22" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="Q22" s="8" t="s">
+      <c r="Q22" s="9" t="s">
         <v>258</v>
       </c>
       <c r="R22" s="2"/>
@@ -32448,10 +32471,10 @@
       <c r="M23" s="2">
         <v>45</v>
       </c>
-      <c r="P23" s="8" t="s">
+      <c r="P23" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="Q23" s="8" t="s">
+      <c r="Q23" s="6" t="s">
         <v>259</v>
       </c>
       <c r="R23" s="2" t="s">
@@ -32498,10 +32521,10 @@
       <c r="M24" s="2">
         <v>45</v>
       </c>
-      <c r="P24" s="8" t="s">
+      <c r="P24" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="Q24" s="8" t="s">
+      <c r="Q24" s="6" t="s">
         <v>260</v>
       </c>
       <c r="R24" s="2" t="s">
@@ -32548,10 +32571,10 @@
       <c r="M25" s="2">
         <v>46</v>
       </c>
-      <c r="P25" s="8" t="s">
+      <c r="P25" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="Q25" s="8" t="s">
+      <c r="Q25" s="6" t="s">
         <v>261</v>
       </c>
       <c r="R25" s="2" t="s">
@@ -32598,10 +32621,10 @@
       <c r="M26" s="2">
         <v>46</v>
       </c>
-      <c r="P26" s="8" t="s">
+      <c r="P26" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="Q26" s="8" t="s">
+      <c r="Q26" s="6" t="s">
         <v>262</v>
       </c>
       <c r="R26" s="2" t="s">
@@ -32648,10 +32671,10 @@
       <c r="M27" s="2">
         <v>46</v>
       </c>
-      <c r="P27" s="8" t="s">
+      <c r="P27" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="Q27" s="8" t="s">
+      <c r="Q27" s="6" t="s">
         <v>263</v>
       </c>
       <c r="R27" s="2" t="s">
@@ -32698,10 +32721,10 @@
       <c r="M28" s="2">
         <v>47</v>
       </c>
-      <c r="P28" s="8" t="s">
+      <c r="P28" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="Q28" s="8" t="s">
+      <c r="Q28" s="6" t="s">
         <v>264</v>
       </c>
       <c r="R28" s="2" t="s">
@@ -32748,10 +32771,10 @@
       <c r="M29" s="2">
         <v>47</v>
       </c>
-      <c r="P29" s="8" t="s">
+      <c r="P29" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="Q29" s="8" t="s">
+      <c r="Q29" s="6" t="s">
         <v>265</v>
       </c>
       <c r="R29" s="2" t="s">
@@ -32798,10 +32821,10 @@
       <c r="M30" s="2">
         <v>47</v>
       </c>
-      <c r="P30" s="8" t="s">
+      <c r="P30" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="Q30" s="8" t="s">
+      <c r="Q30" s="6" t="s">
         <v>266</v>
       </c>
       <c r="R30" s="2" t="s">
@@ -32848,10 +32871,10 @@
       <c r="M31" s="2">
         <v>48</v>
       </c>
-      <c r="P31" s="8" t="s">
+      <c r="P31" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="Q31" s="8" t="s">
+      <c r="Q31" s="6" t="s">
         <v>267</v>
       </c>
       <c r="R31" s="2" t="s">
@@ -32898,10 +32921,10 @@
       <c r="M32" s="2">
         <v>48</v>
       </c>
-      <c r="P32" s="8" t="s">
+      <c r="P32" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="Q32" s="8" t="s">
+      <c r="Q32" s="6" t="s">
         <v>268</v>
       </c>
       <c r="R32" s="2" t="s">
@@ -32948,10 +32971,10 @@
       <c r="M33" s="2">
         <v>48</v>
       </c>
-      <c r="P33" s="8" t="s">
+      <c r="P33" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="Q33" s="8" t="s">
+      <c r="Q33" s="6" t="s">
         <v>269</v>
       </c>
       <c r="R33" s="2" t="s">
@@ -32998,10 +33021,10 @@
       <c r="M34" s="2">
         <v>49</v>
       </c>
-      <c r="P34" s="8" t="s">
+      <c r="P34" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="Q34" s="8" t="s">
+      <c r="Q34" s="6" t="s">
         <v>270</v>
       </c>
       <c r="R34" s="2" t="s">
@@ -33048,10 +33071,10 @@
       <c r="M35" s="2">
         <v>50</v>
       </c>
-      <c r="P35" s="8" t="s">
+      <c r="P35" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="Q35" s="8" t="s">
+      <c r="Q35" s="6" t="s">
         <v>271</v>
       </c>
       <c r="R35" s="2" t="s">
@@ -33098,10 +33121,10 @@
       <c r="M36" s="2">
         <v>50</v>
       </c>
-      <c r="P36" s="8" t="s">
+      <c r="P36" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="Q36" s="8" t="s">
+      <c r="Q36" s="6" t="s">
         <v>272</v>
       </c>
       <c r="R36" s="2" t="s">
@@ -33148,10 +33171,10 @@
       <c r="M37" s="2">
         <v>52</v>
       </c>
-      <c r="P37" s="8" t="s">
+      <c r="P37" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="Q37" s="8" t="s">
+      <c r="Q37" s="6" t="s">
         <v>273</v>
       </c>
       <c r="R37" s="2" t="s">
@@ -33198,10 +33221,10 @@
       <c r="M38" s="2">
         <v>52</v>
       </c>
-      <c r="P38" s="8" t="s">
+      <c r="P38" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="Q38" s="8" t="s">
+      <c r="Q38" s="6" t="s">
         <v>274</v>
       </c>
       <c r="R38" s="2" t="s">
@@ -33248,10 +33271,10 @@
       <c r="M39" s="2">
         <v>53</v>
       </c>
-      <c r="P39" s="8" t="s">
+      <c r="P39" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="Q39" s="8" t="s">
+      <c r="Q39" s="6" t="s">
         <v>275</v>
       </c>
       <c r="R39" s="2" t="s">
@@ -33298,10 +33321,10 @@
       <c r="M40" s="2">
         <v>53</v>
       </c>
-      <c r="P40" s="8" t="s">
+      <c r="P40" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="Q40" s="8" t="s">
+      <c r="Q40" s="6" t="s">
         <v>276</v>
       </c>
       <c r="R40" s="2" t="s">
@@ -33348,10 +33371,10 @@
       <c r="M41" s="2">
         <v>53</v>
       </c>
-      <c r="P41" s="8" t="s">
+      <c r="P41" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="Q41" s="8" t="s">
+      <c r="Q41" s="6" t="s">
         <v>277</v>
       </c>
       <c r="R41" s="2" t="s">
@@ -33398,10 +33421,10 @@
       <c r="M42" s="2">
         <v>55</v>
       </c>
-      <c r="P42" s="8" t="s">
+      <c r="P42" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="Q42" s="8" t="s">
+      <c r="Q42" s="6" t="s">
         <v>278</v>
       </c>
       <c r="R42" s="2" t="s">
@@ -33448,10 +33471,10 @@
       <c r="M43" s="2">
         <v>57</v>
       </c>
-      <c r="P43" s="8" t="s">
+      <c r="P43" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="Q43" s="8" t="s">
+      <c r="Q43" s="6" t="s">
         <v>279</v>
       </c>
       <c r="R43" s="2" t="s">
@@ -33498,10 +33521,10 @@
       <c r="M44" s="2">
         <v>57</v>
       </c>
-      <c r="P44" s="8" t="s">
+      <c r="P44" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="Q44" s="8" t="s">
+      <c r="Q44" s="6" t="s">
         <v>280</v>
       </c>
       <c r="R44" s="2" t="s">
@@ -33548,10 +33571,10 @@
       <c r="M45" s="2">
         <v>58</v>
       </c>
-      <c r="P45" s="8" t="s">
+      <c r="P45" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="Q45" s="8" t="s">
+      <c r="Q45" s="6" t="s">
         <v>281</v>
       </c>
       <c r="R45" s="2" t="s">
@@ -33598,10 +33621,10 @@
       <c r="M46" s="2">
         <v>58</v>
       </c>
-      <c r="P46" s="8" t="s">
+      <c r="P46" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="Q46" s="8" t="s">
+      <c r="Q46" s="6" t="s">
         <v>282</v>
       </c>
       <c r="R46" s="2" t="s">
@@ -33648,10 +33671,10 @@
       <c r="M47" s="2">
         <v>58</v>
       </c>
-      <c r="P47" s="8" t="s">
+      <c r="P47" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="Q47" s="8" t="s">
+      <c r="Q47" s="6" t="s">
         <v>283</v>
       </c>
       <c r="R47" s="2" t="s">
@@ -33698,10 +33721,10 @@
       <c r="M48" s="2">
         <v>59</v>
       </c>
-      <c r="P48" s="8" t="s">
+      <c r="P48" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="Q48" s="8" t="s">
+      <c r="Q48" s="6" t="s">
         <v>284</v>
       </c>
       <c r="R48" s="2" t="s">
@@ -33748,10 +33771,10 @@
       <c r="M49" s="2">
         <v>64</v>
       </c>
-      <c r="P49" s="8" t="s">
+      <c r="P49" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="Q49" s="8" t="s">
+      <c r="Q49" s="6" t="s">
         <v>285</v>
       </c>
       <c r="R49" s="2" t="s">
@@ -33798,10 +33821,10 @@
       <c r="M50" s="2">
         <v>64</v>
       </c>
-      <c r="P50" s="8" t="s">
+      <c r="P50" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="Q50" s="8" t="s">
+      <c r="Q50" s="6" t="s">
         <v>286</v>
       </c>
       <c r="R50" s="2" t="s">
@@ -33848,10 +33871,10 @@
       <c r="M51" s="2">
         <v>65</v>
       </c>
-      <c r="P51" s="8" t="s">
+      <c r="P51" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="Q51" s="8" t="s">
+      <c r="Q51" s="6" t="s">
         <v>287</v>
       </c>
       <c r="R51" s="2" t="s">
@@ -33898,10 +33921,10 @@
       <c r="M52" s="2">
         <v>67</v>
       </c>
-      <c r="P52" s="8" t="s">
+      <c r="P52" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="Q52" s="8" t="s">
+      <c r="Q52" s="6" t="s">
         <v>288</v>
       </c>
       <c r="R52" s="2" t="s">
@@ -33948,10 +33971,10 @@
       <c r="M53" s="2">
         <v>68</v>
       </c>
-      <c r="P53" s="8" t="s">
+      <c r="P53" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="Q53" s="8" t="s">
+      <c r="Q53" s="6" t="s">
         <v>289</v>
       </c>
       <c r="R53" s="2" t="s">
@@ -33998,10 +34021,10 @@
       <c r="M54" s="2">
         <v>69</v>
       </c>
-      <c r="P54" s="8" t="s">
+      <c r="P54" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="Q54" s="8" t="s">
+      <c r="Q54" s="6" t="s">
         <v>290</v>
       </c>
       <c r="R54" s="2" t="s">
@@ -34048,10 +34071,10 @@
       <c r="M55" s="2">
         <v>74</v>
       </c>
-      <c r="P55" s="8" t="s">
+      <c r="P55" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="Q55" s="8" t="s">
+      <c r="Q55" s="6" t="s">
         <v>291</v>
       </c>
       <c r="R55" s="2" t="s">
@@ -34098,10 +34121,10 @@
       <c r="M56" s="2">
         <v>80</v>
       </c>
-      <c r="P56" s="8" t="s">
+      <c r="P56" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="Q56" s="8" t="s">
+      <c r="Q56" s="6" t="s">
         <v>292</v>
       </c>
       <c r="R56" s="2" t="s">
@@ -34112,10 +34135,10 @@
       </c>
     </row>
     <row r="57" spans="1:19">
-      <c r="P57" s="8" t="s">
+      <c r="P57" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="Q57" s="8" t="s">
+      <c r="Q57" s="6" t="s">
         <v>293</v>
       </c>
       <c r="R57" s="2" t="s">
@@ -34126,10 +34149,10 @@
       </c>
     </row>
     <row r="58" spans="1:19">
-      <c r="P58" s="8" t="s">
+      <c r="P58" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="Q58" s="8" t="s">
+      <c r="Q58" s="6" t="s">
         <v>294</v>
       </c>
       <c r="R58" s="2" t="s">
@@ -34140,10 +34163,10 @@
       </c>
     </row>
     <row r="59" spans="1:19">
-      <c r="P59" s="8" t="s">
+      <c r="P59" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="Q59" s="8" t="s">
+      <c r="Q59" s="6" t="s">
         <v>295</v>
       </c>
       <c r="R59" s="2" t="s">
@@ -34154,21 +34177,21 @@
       </c>
     </row>
     <row r="60" spans="1:19">
-      <c r="P60" s="8" t="s">
+      <c r="P60" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="Q60" s="7" t="s">
         <v>296</v>
-      </c>
-      <c r="Q60" s="8" t="s">
-        <v>297</v>
       </c>
       <c r="R60" s="2"/>
       <c r="S60" s="2"/>
     </row>
     <row r="61" spans="1:19">
-      <c r="P61" s="8" t="s">
+      <c r="P61" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="Q61" s="8" t="s">
-        <v>298</v>
+      <c r="Q61" s="6" t="s">
+        <v>297</v>
       </c>
       <c r="R61" s="2" t="s">
         <v>119</v>
@@ -34178,11 +34201,11 @@
       </c>
     </row>
     <row r="62" spans="1:19">
-      <c r="P62" s="8" t="s">
+      <c r="P62" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="Q62" s="8" t="s">
-        <v>299</v>
+      <c r="Q62" s="6" t="s">
+        <v>298</v>
       </c>
       <c r="R62" s="2" t="s">
         <v>121</v>
@@ -34192,11 +34215,11 @@
       </c>
     </row>
     <row r="63" spans="1:19">
-      <c r="P63" s="8" t="s">
+      <c r="P63" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="Q63" s="8" t="s">
-        <v>300</v>
+      <c r="Q63" s="6" t="s">
+        <v>299</v>
       </c>
       <c r="R63" s="2" t="s">
         <v>123</v>
@@ -34206,11 +34229,11 @@
       </c>
     </row>
     <row r="64" spans="1:19">
-      <c r="P64" s="8" t="s">
+      <c r="P64" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="Q64" s="8" t="s">
-        <v>301</v>
+      <c r="Q64" s="6" t="s">
+        <v>300</v>
       </c>
       <c r="R64" s="2" t="s">
         <v>125</v>
@@ -34220,11 +34243,11 @@
       </c>
     </row>
     <row r="65" spans="16:19">
-      <c r="P65" s="8" t="s">
+      <c r="P65" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="Q65" s="8" t="s">
-        <v>302</v>
+      <c r="Q65" s="6" t="s">
+        <v>301</v>
       </c>
       <c r="R65" s="2" t="s">
         <v>127</v>
@@ -34234,11 +34257,11 @@
       </c>
     </row>
     <row r="66" spans="16:19">
-      <c r="P66" s="8" t="s">
+      <c r="P66" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="Q66" s="8" t="s">
-        <v>303</v>
+      <c r="Q66" s="6" t="s">
+        <v>302</v>
       </c>
       <c r="R66" s="2" t="s">
         <v>129</v>
@@ -34248,11 +34271,11 @@
       </c>
     </row>
     <row r="67" spans="16:19">
-      <c r="P67" s="8" t="s">
+      <c r="P67" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="Q67" s="8" t="s">
-        <v>304</v>
+      <c r="Q67" s="6" t="s">
+        <v>303</v>
       </c>
       <c r="R67" s="2" t="s">
         <v>131</v>
@@ -34262,11 +34285,11 @@
       </c>
     </row>
     <row r="68" spans="16:19">
-      <c r="P68" s="8" t="s">
+      <c r="P68" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="Q68" s="8" t="s">
-        <v>305</v>
+      <c r="Q68" s="6" t="s">
+        <v>304</v>
       </c>
       <c r="R68" s="2" t="s">
         <v>133</v>
@@ -34276,11 +34299,11 @@
       </c>
     </row>
     <row r="69" spans="16:19">
-      <c r="P69" s="8" t="s">
+      <c r="P69" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="Q69" s="8" t="s">
-        <v>306</v>
+      <c r="Q69" s="6" t="s">
+        <v>305</v>
       </c>
       <c r="R69" s="2" t="s">
         <v>135</v>
@@ -34290,11 +34313,11 @@
       </c>
     </row>
     <row r="70" spans="16:19">
-      <c r="P70" s="8" t="s">
+      <c r="P70" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="Q70" s="8" t="s">
-        <v>307</v>
+      <c r="Q70" s="6" t="s">
+        <v>306</v>
       </c>
       <c r="R70" s="2" t="s">
         <v>137</v>
@@ -34304,11 +34327,11 @@
       </c>
     </row>
     <row r="71" spans="16:19">
-      <c r="P71" s="8" t="s">
+      <c r="P71" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="Q71" s="8" t="s">
-        <v>308</v>
+      <c r="Q71" s="6" t="s">
+        <v>307</v>
       </c>
       <c r="R71" s="2" t="s">
         <v>139</v>
@@ -34318,11 +34341,11 @@
       </c>
     </row>
     <row r="72" spans="16:19">
-      <c r="P72" s="8" t="s">
+      <c r="P72" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="Q72" s="8" t="s">
-        <v>309</v>
+      <c r="Q72" s="6" t="s">
+        <v>308</v>
       </c>
       <c r="R72" s="2" t="s">
         <v>141</v>
@@ -34332,11 +34355,11 @@
       </c>
     </row>
     <row r="73" spans="16:19">
-      <c r="P73" s="8" t="s">
+      <c r="P73" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="Q73" s="8" t="s">
-        <v>310</v>
+      <c r="Q73" s="6" t="s">
+        <v>309</v>
       </c>
       <c r="R73" s="2" t="s">
         <v>143</v>
@@ -34346,21 +34369,21 @@
       </c>
     </row>
     <row r="74" spans="16:19">
-      <c r="P74" s="8" t="s">
+      <c r="P74" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q74" s="7" t="s">
         <v>311</v>
-      </c>
-      <c r="Q74" s="8" t="s">
-        <v>312</v>
       </c>
       <c r="R74" s="2"/>
       <c r="S74" s="2"/>
     </row>
     <row r="75" spans="16:19">
-      <c r="P75" s="8" t="s">
+      <c r="P75" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="Q75" s="8" t="s">
-        <v>313</v>
+      <c r="Q75" s="6" t="s">
+        <v>312</v>
       </c>
       <c r="R75" s="2" t="s">
         <v>145</v>
@@ -34370,11 +34393,11 @@
       </c>
     </row>
     <row r="76" spans="16:19">
-      <c r="P76" s="8" t="s">
+      <c r="P76" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="Q76" s="8" t="s">
-        <v>314</v>
+      <c r="Q76" s="6" t="s">
+        <v>313</v>
       </c>
       <c r="R76" s="2" t="s">
         <v>147</v>
@@ -34384,11 +34407,11 @@
       </c>
     </row>
     <row r="77" spans="16:19">
-      <c r="P77" s="8" t="s">
+      <c r="P77" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="Q77" s="8" t="s">
-        <v>315</v>
+      <c r="Q77" s="6" t="s">
+        <v>314</v>
       </c>
       <c r="R77" s="2" t="s">
         <v>149</v>
@@ -34398,11 +34421,11 @@
       </c>
     </row>
     <row r="78" spans="16:19">
-      <c r="P78" s="8" t="s">
+      <c r="P78" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="Q78" s="8" t="s">
-        <v>316</v>
+      <c r="Q78" s="6" t="s">
+        <v>315</v>
       </c>
       <c r="R78" s="2" t="s">
         <v>151</v>
@@ -34412,11 +34435,11 @@
       </c>
     </row>
     <row r="79" spans="16:19">
-      <c r="P79" s="8" t="s">
+      <c r="P79" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="Q79" s="8" t="s">
-        <v>317</v>
+      <c r="Q79" s="6" t="s">
+        <v>316</v>
       </c>
       <c r="R79" s="2" t="s">
         <v>153</v>
@@ -34426,11 +34449,11 @@
       </c>
     </row>
     <row r="80" spans="16:19">
-      <c r="P80" s="8" t="s">
+      <c r="P80" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="Q80" s="8" t="s">
-        <v>318</v>
+      <c r="Q80" s="6" t="s">
+        <v>317</v>
       </c>
       <c r="R80" s="2" t="s">
         <v>155</v>
@@ -34440,11 +34463,11 @@
       </c>
     </row>
     <row r="81" spans="16:19">
-      <c r="P81" s="8" t="s">
+      <c r="P81" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="Q81" s="8" t="s">
-        <v>319</v>
+      <c r="Q81" s="6" t="s">
+        <v>318</v>
       </c>
       <c r="R81" s="2" t="s">
         <v>157</v>
@@ -34454,21 +34477,25 @@
       </c>
     </row>
     <row r="82" spans="16:19">
-      <c r="P82" s="8" t="s">
+      <c r="P82" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="Q82" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="Q82" s="8" t="s">
+      <c r="R82" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="S82" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="83" spans="16:19">
+      <c r="P83" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q83" s="6" t="s">
         <v>321</v>
-      </c>
-      <c r="R82" s="2"/>
-      <c r="S82" s="2"/>
-    </row>
-    <row r="83" spans="16:19">
-      <c r="P83" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q83" s="8" t="s">
-        <v>322</v>
       </c>
       <c r="R83" s="2" t="s">
         <v>159</v>
@@ -34478,11 +34505,11 @@
       </c>
     </row>
     <row r="84" spans="16:19">
-      <c r="P84" s="8" t="s">
+      <c r="P84" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="Q84" s="8" t="s">
-        <v>323</v>
+      <c r="Q84" s="6" t="s">
+        <v>322</v>
       </c>
       <c r="R84" s="2" t="s">
         <v>161</v>
@@ -34492,11 +34519,11 @@
       </c>
     </row>
     <row r="85" spans="16:19">
-      <c r="P85" s="8" t="s">
+      <c r="P85" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="Q85" s="8" t="s">
-        <v>324</v>
+      <c r="Q85" s="6" t="s">
+        <v>323</v>
       </c>
       <c r="R85" s="2" t="s">
         <v>163</v>
@@ -34506,11 +34533,11 @@
       </c>
     </row>
     <row r="86" spans="16:19">
-      <c r="P86" s="8" t="s">
+      <c r="P86" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="Q86" s="8" t="s">
-        <v>325</v>
+      <c r="Q86" s="6" t="s">
+        <v>324</v>
       </c>
       <c r="R86" s="2" t="s">
         <v>165</v>
@@ -34520,11 +34547,11 @@
       </c>
     </row>
     <row r="87" spans="16:19">
-      <c r="P87" s="8" t="s">
+      <c r="P87" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="Q87" s="8" t="s">
-        <v>326</v>
+      <c r="Q87" s="6" t="s">
+        <v>325</v>
       </c>
       <c r="R87" s="2" t="s">
         <v>167</v>
@@ -34534,11 +34561,11 @@
       </c>
     </row>
     <row r="88" spans="16:19">
-      <c r="P88" s="8" t="s">
+      <c r="P88" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="Q88" s="8" t="s">
-        <v>327</v>
+      <c r="Q88" s="6" t="s">
+        <v>326</v>
       </c>
       <c r="R88" s="2" t="s">
         <v>169</v>
@@ -34548,11 +34575,11 @@
       </c>
     </row>
     <row r="89" spans="16:19">
-      <c r="P89" s="8" t="s">
+      <c r="P89" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="Q89" s="8" t="s">
-        <v>328</v>
+      <c r="Q89" s="6" t="s">
+        <v>327</v>
       </c>
       <c r="R89" s="2" t="s">
         <v>171</v>
@@ -34562,11 +34589,11 @@
       </c>
     </row>
     <row r="90" spans="16:19">
-      <c r="P90" s="8" t="s">
+      <c r="P90" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="Q90" s="8" t="s">
-        <v>329</v>
+      <c r="Q90" s="6" t="s">
+        <v>328</v>
       </c>
       <c r="R90" s="2" t="s">
         <v>173</v>
@@ -34576,11 +34603,11 @@
       </c>
     </row>
     <row r="91" spans="16:19">
-      <c r="P91" s="8" t="s">
+      <c r="P91" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="Q91" s="8" t="s">
-        <v>330</v>
+      <c r="Q91" s="6" t="s">
+        <v>329</v>
       </c>
       <c r="R91" s="2" t="s">
         <v>175</v>
@@ -34590,11 +34617,11 @@
       </c>
     </row>
     <row r="92" spans="16:19">
-      <c r="P92" s="8" t="s">
+      <c r="P92" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="Q92" s="8" t="s">
-        <v>331</v>
+      <c r="Q92" s="6" t="s">
+        <v>330</v>
       </c>
       <c r="R92" s="2" t="s">
         <v>177</v>
@@ -34604,11 +34631,11 @@
       </c>
     </row>
     <row r="93" spans="16:19">
-      <c r="P93" s="8" t="s">
+      <c r="P93" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="Q93" s="8" t="s">
-        <v>332</v>
+      <c r="Q93" s="6" t="s">
+        <v>331</v>
       </c>
       <c r="R93" s="2" t="s">
         <v>179</v>
@@ -34618,11 +34645,11 @@
       </c>
     </row>
     <row r="94" spans="16:19">
-      <c r="P94" s="8" t="s">
+      <c r="P94" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="Q94" s="8" t="s">
-        <v>333</v>
+      <c r="Q94" s="6" t="s">
+        <v>332</v>
       </c>
       <c r="R94" s="2" t="s">
         <v>181</v>
@@ -34632,11 +34659,11 @@
       </c>
     </row>
     <row r="95" spans="16:19">
-      <c r="P95" s="8" t="s">
+      <c r="P95" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="Q95" s="8" t="s">
-        <v>334</v>
+      <c r="Q95" s="6" t="s">
+        <v>333</v>
       </c>
       <c r="R95" s="2" t="s">
         <v>183</v>
@@ -34646,11 +34673,11 @@
       </c>
     </row>
     <row r="96" spans="16:19">
-      <c r="P96" s="8" t="s">
+      <c r="P96" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="Q96" s="8" t="s">
-        <v>335</v>
+      <c r="Q96" s="6" t="s">
+        <v>334</v>
       </c>
       <c r="R96" s="2" t="s">
         <v>185</v>
@@ -34660,11 +34687,11 @@
       </c>
     </row>
     <row r="97" spans="16:19">
-      <c r="P97" s="8" t="s">
+      <c r="P97" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="Q97" s="8" t="s">
-        <v>336</v>
+      <c r="Q97" s="6" t="s">
+        <v>335</v>
       </c>
       <c r="R97" s="2" t="s">
         <v>187</v>
@@ -34674,11 +34701,11 @@
       </c>
     </row>
     <row r="98" spans="16:19">
-      <c r="P98" s="8" t="s">
+      <c r="P98" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="Q98" s="8" t="s">
-        <v>337</v>
+      <c r="Q98" s="6" t="s">
+        <v>336</v>
       </c>
       <c r="R98" s="2" t="s">
         <v>189</v>
@@ -34688,11 +34715,11 @@
       </c>
     </row>
     <row r="99" spans="16:19">
-      <c r="P99" s="8" t="s">
+      <c r="P99" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="Q99" s="8" t="s">
-        <v>338</v>
+      <c r="Q99" s="6" t="s">
+        <v>337</v>
       </c>
       <c r="R99" s="2" t="s">
         <v>191</v>
@@ -34702,11 +34729,11 @@
       </c>
     </row>
     <row r="100" spans="16:19">
-      <c r="P100" s="8" t="s">
+      <c r="P100" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="Q100" s="8" t="s">
-        <v>339</v>
+      <c r="Q100" s="6" t="s">
+        <v>338</v>
       </c>
       <c r="R100" s="2" t="s">
         <v>193</v>
@@ -34716,11 +34743,11 @@
       </c>
     </row>
     <row r="101" spans="16:19">
-      <c r="P101" s="8" t="s">
+      <c r="P101" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="Q101" s="8" t="s">
-        <v>340</v>
+      <c r="Q101" s="6" t="s">
+        <v>339</v>
       </c>
       <c r="R101" s="2" t="s">
         <v>195</v>
@@ -34730,11 +34757,11 @@
       </c>
     </row>
     <row r="102" spans="16:19">
-      <c r="P102" s="8" t="s">
+      <c r="P102" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="Q102" s="8" t="s">
-        <v>341</v>
+      <c r="Q102" s="6" t="s">
+        <v>340</v>
       </c>
       <c r="R102" s="2" t="s">
         <v>197</v>
@@ -34744,11 +34771,11 @@
       </c>
     </row>
     <row r="103" spans="16:19">
-      <c r="P103" s="8" t="s">
+      <c r="P103" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="Q103" s="8" t="s">
-        <v>342</v>
+      <c r="Q103" s="6" t="s">
+        <v>341</v>
       </c>
       <c r="R103" s="2" t="s">
         <v>199</v>
@@ -34758,11 +34785,11 @@
       </c>
     </row>
     <row r="104" spans="16:19">
-      <c r="P104" s="8" t="s">
+      <c r="P104" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="Q104" s="8" t="s">
-        <v>343</v>
+      <c r="Q104" s="6" t="s">
+        <v>342</v>
       </c>
       <c r="R104" s="2" t="s">
         <v>201</v>
@@ -34772,11 +34799,11 @@
       </c>
     </row>
     <row r="105" spans="16:19">
-      <c r="P105" s="8" t="s">
+      <c r="P105" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="Q105" s="8" t="s">
-        <v>344</v>
+      <c r="Q105" s="6" t="s">
+        <v>343</v>
       </c>
       <c r="R105" s="2" t="s">
         <v>203</v>
@@ -34786,11 +34813,11 @@
       </c>
     </row>
     <row r="106" spans="16:19">
-      <c r="P106" s="8" t="s">
+      <c r="P106" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="Q106" s="8" t="s">
-        <v>345</v>
+      <c r="Q106" s="6" t="s">
+        <v>344</v>
       </c>
       <c r="R106" s="2" t="s">
         <v>205</v>
@@ -34800,11 +34827,11 @@
       </c>
     </row>
     <row r="107" spans="16:19">
-      <c r="P107" s="8" t="s">
+      <c r="P107" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="Q107" s="8" t="s">
-        <v>346</v>
+      <c r="Q107" s="6" t="s">
+        <v>345</v>
       </c>
       <c r="R107" s="2" t="s">
         <v>207</v>
@@ -34814,11 +34841,11 @@
       </c>
     </row>
     <row r="108" spans="16:19">
-      <c r="P108" s="8" t="s">
+      <c r="P108" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="Q108" s="8" t="s">
-        <v>347</v>
+      <c r="Q108" s="6" t="s">
+        <v>346</v>
       </c>
       <c r="R108" s="2" t="s">
         <v>209</v>
@@ -34828,11 +34855,11 @@
       </c>
     </row>
     <row r="109" spans="16:19">
-      <c r="P109" s="8" t="s">
+      <c r="P109" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="Q109" s="8" t="s">
-        <v>348</v>
+      <c r="Q109" s="6" t="s">
+        <v>347</v>
       </c>
       <c r="R109" s="2" t="s">
         <v>211</v>
@@ -34842,11 +34869,11 @@
       </c>
     </row>
     <row r="110" spans="16:19">
-      <c r="P110" s="8" t="s">
+      <c r="P110" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="Q110" s="8" t="s">
-        <v>349</v>
+      <c r="Q110" s="6" t="s">
+        <v>348</v>
       </c>
       <c r="R110" s="2" t="s">
         <v>213</v>
@@ -34856,11 +34883,11 @@
       </c>
     </row>
     <row r="111" spans="16:19">
-      <c r="P111" s="8" t="s">
+      <c r="P111" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="Q111" s="8" t="s">
-        <v>350</v>
+      <c r="Q111" s="6" t="s">
+        <v>349</v>
       </c>
       <c r="R111" s="2" t="s">
         <v>215</v>
@@ -34870,11 +34897,11 @@
       </c>
     </row>
     <row r="112" spans="16:19">
-      <c r="P112" s="8" t="s">
+      <c r="P112" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="Q112" s="8" t="s">
-        <v>351</v>
+      <c r="Q112" s="6" t="s">
+        <v>350</v>
       </c>
       <c r="R112" s="2" t="s">
         <v>217</v>
@@ -34884,11 +34911,11 @@
       </c>
     </row>
     <row r="113" spans="16:19">
-      <c r="P113" s="8" t="s">
+      <c r="P113" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="Q113" s="8" t="s">
-        <v>352</v>
+      <c r="Q113" s="6" t="s">
+        <v>351</v>
       </c>
       <c r="R113" s="2" t="s">
         <v>219</v>
@@ -34898,25 +34925,17 @@
       </c>
     </row>
     <row r="114" spans="16:19">
-      <c r="P114" s="8" t="s">
+      <c r="P114" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="Q114" s="8" t="s">
-        <v>353</v>
+      <c r="Q114" s="6" t="s">
+        <v>352</v>
       </c>
       <c r="R114" s="2" t="s">
         <v>221</v>
       </c>
       <c r="S114" s="2" t="s">
         <v>222</v>
-      </c>
-    </row>
-    <row r="115" spans="16:19">
-      <c r="R115" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="S115" s="2" t="s">
-        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>